<commit_message>
Capa Fisica: Caracteristicas y Problemas
</commit_message>
<xml_diff>
--- a/docs/protocols-suite.xlsx
+++ b/docs/protocols-suite.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna1-mj20\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1F206BA-143C-4A75-B0A4-07B68D454023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE3FFCF-5BB8-45A0-8702-C194A7BEAE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{61336F32-1C3D-4908-AE32-B989E9366DB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{61336F32-1C3D-4908-AE32-B989E9366DB6}"/>
   </bookViews>
   <sheets>
     <sheet name="suite" sheetId="1" r:id="rId1"/>
+    <sheet name="unidades" sheetId="2" r:id="rId2"/>
+    <sheet name="fisica" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="183">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -109,6 +111,480 @@
   </si>
   <si>
     <t>HTTP - HTTPS - FTP - SFTP - TFTP - POP - IMAP - SMTP - SSH - TELNET - DNS - DHCP</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>binary digit</t>
+  </si>
+  <si>
+    <t>Almacenamiento</t>
+  </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>8 bits</t>
+  </si>
+  <si>
+    <t>unidad</t>
+  </si>
+  <si>
+    <t>equivalencia</t>
+  </si>
+  <si>
+    <t>exponente</t>
+  </si>
+  <si>
+    <t>10^0</t>
+  </si>
+  <si>
+    <t>1000b</t>
+  </si>
+  <si>
+    <t>10^3</t>
+  </si>
+  <si>
+    <t>Megabyte</t>
+  </si>
+  <si>
+    <t>1000Kb</t>
+  </si>
+  <si>
+    <t>10^6</t>
+  </si>
+  <si>
+    <t>10^9</t>
+  </si>
+  <si>
+    <t>10^12</t>
+  </si>
+  <si>
+    <t>10^15</t>
+  </si>
+  <si>
+    <t>10^18</t>
+  </si>
+  <si>
+    <t>10^21</t>
+  </si>
+  <si>
+    <t>10^24</t>
+  </si>
+  <si>
+    <t>10^27</t>
+  </si>
+  <si>
+    <t>10^30</t>
+  </si>
+  <si>
+    <t>10^33</t>
+  </si>
+  <si>
+    <t>Gigabyte</t>
+  </si>
+  <si>
+    <t>1000Mb</t>
+  </si>
+  <si>
+    <t>Terabyte</t>
+  </si>
+  <si>
+    <t>1000Gb</t>
+  </si>
+  <si>
+    <t>Petabyte</t>
+  </si>
+  <si>
+    <t>1000Tb</t>
+  </si>
+  <si>
+    <t>Exabyte</t>
+  </si>
+  <si>
+    <t>1000Pb</t>
+  </si>
+  <si>
+    <t>Zettabyte</t>
+  </si>
+  <si>
+    <t>1000Xb</t>
+  </si>
+  <si>
+    <t>Yotabyte</t>
+  </si>
+  <si>
+    <t>1000Zb</t>
+  </si>
+  <si>
+    <t>Brontobyte</t>
+  </si>
+  <si>
+    <t>1000Yb</t>
+  </si>
+  <si>
+    <t>Geopbyte</t>
+  </si>
+  <si>
+    <t>Sangan</t>
+  </si>
+  <si>
+    <t>1000Bb</t>
+  </si>
+  <si>
+    <t>1000Geb</t>
+  </si>
+  <si>
+    <t>Ancho de Banda</t>
+  </si>
+  <si>
+    <t>exponencia</t>
+  </si>
+  <si>
+    <t>bit/s</t>
+  </si>
+  <si>
+    <t>transmision</t>
+  </si>
+  <si>
+    <t>Kilobyte</t>
+  </si>
+  <si>
+    <t>1000bps</t>
+  </si>
+  <si>
+    <t>1000kbps</t>
+  </si>
+  <si>
+    <t>1000mbps</t>
+  </si>
+  <si>
+    <t>1000gbps</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>hertz</t>
+  </si>
+  <si>
+    <t>1 ciclo/s</t>
+  </si>
+  <si>
+    <t>1000Hz</t>
+  </si>
+  <si>
+    <t>1000KHz</t>
+  </si>
+  <si>
+    <t>1000MHz</t>
+  </si>
+  <si>
+    <t>1000GHz</t>
+  </si>
+  <si>
+    <t>Kilobit/s</t>
+  </si>
+  <si>
+    <t>Megabit/s</t>
+  </si>
+  <si>
+    <t>Gigabit/s</t>
+  </si>
+  <si>
+    <t>Terabit/s</t>
+  </si>
+  <si>
+    <t>Kilohertz</t>
+  </si>
+  <si>
+    <t>Megahertz</t>
+  </si>
+  <si>
+    <t>Gigahertz</t>
+  </si>
+  <si>
+    <t>Terahertz</t>
+  </si>
+  <si>
+    <t>TIA</t>
+  </si>
+  <si>
+    <t>TIA-568A</t>
+  </si>
+  <si>
+    <t>TIA-568B</t>
+  </si>
+  <si>
+    <t>b.verde</t>
+  </si>
+  <si>
+    <t>verde</t>
+  </si>
+  <si>
+    <t>b.naranja</t>
+  </si>
+  <si>
+    <t>naranja</t>
+  </si>
+  <si>
+    <t>azul</t>
+  </si>
+  <si>
+    <t>b.azul</t>
+  </si>
+  <si>
+    <t>marron</t>
+  </si>
+  <si>
+    <t>b.marron</t>
+  </si>
+  <si>
+    <t>tx</t>
+  </si>
+  <si>
+    <t>rx</t>
+  </si>
+  <si>
+    <t>HalfDuplex</t>
+  </si>
+  <si>
+    <t>FullDuplex</t>
+  </si>
+  <si>
+    <t>Simplex</t>
+  </si>
+  <si>
+    <t>envia y recibe</t>
+  </si>
+  <si>
+    <t>envia o recibe</t>
+  </si>
+  <si>
+    <t>solo envia</t>
+  </si>
+  <si>
+    <t>Full/FullDuplex</t>
+  </si>
+  <si>
+    <t>envian y reciben</t>
+  </si>
+  <si>
+    <t>radiodifusion</t>
+  </si>
+  <si>
+    <t>telefonia</t>
+  </si>
+  <si>
+    <t>comunicador</t>
+  </si>
+  <si>
+    <t>llamada grupal</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>CARRIER</t>
+  </si>
+  <si>
+    <t>Amplitud Modulada</t>
+  </si>
+  <si>
+    <t>Frecuencia Modulada</t>
+  </si>
+  <si>
+    <t>Modulacion de Fase</t>
+  </si>
+  <si>
+    <t>Señal Portadora</t>
+  </si>
+  <si>
+    <t>Monomodo</t>
+  </si>
+  <si>
+    <t>Multimodo</t>
+  </si>
+  <si>
+    <t>Laser</t>
+  </si>
+  <si>
+    <t>L.E.D.</t>
+  </si>
+  <si>
+    <t>Tecnologia</t>
+  </si>
+  <si>
+    <t>Usos</t>
+  </si>
+  <si>
+    <t>Empresarial</t>
+  </si>
+  <si>
+    <t>FTTH (Hogareño)</t>
+  </si>
+  <si>
+    <t>Distancia</t>
+  </si>
+  <si>
+    <t>200km</t>
+  </si>
+  <si>
+    <t>2km</t>
+  </si>
+  <si>
+    <t>Ventajas</t>
+  </si>
+  <si>
+    <t>Contras</t>
+  </si>
+  <si>
+    <t>Electronica</t>
+  </si>
+  <si>
+    <t>Economica</t>
+  </si>
+  <si>
+    <t>Nucleo</t>
+  </si>
+  <si>
+    <t>60 nanometros</t>
+  </si>
+  <si>
+    <t>9 nanometros</t>
+  </si>
+  <si>
+    <t>Capacidad</t>
+  </si>
+  <si>
+    <t>10Gbps</t>
+  </si>
+  <si>
+    <t>100Gbps</t>
+  </si>
+  <si>
+    <t>Significado</t>
+  </si>
+  <si>
+    <t>SMF(Single Mode)</t>
+  </si>
+  <si>
+    <t>MMF (MultiMode)</t>
+  </si>
+  <si>
+    <t>Fibra</t>
+  </si>
+  <si>
+    <t>conectores</t>
+  </si>
+  <si>
+    <t>terminaciones</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>Suscriber Connector</t>
+  </si>
+  <si>
+    <t>Ferrule Conector</t>
+  </si>
+  <si>
+    <t>Lucent Conector</t>
+  </si>
+  <si>
+    <t>Straight Tip</t>
+  </si>
+  <si>
+    <t>Physical Contact</t>
+  </si>
+  <si>
+    <t>Angled Physical Contact</t>
+  </si>
+  <si>
+    <t>Ultra Physical Contact</t>
+  </si>
+  <si>
+    <t>Largo de la Onda</t>
+  </si>
+  <si>
+    <t>Cantidad de Ciclos</t>
+  </si>
+  <si>
+    <t>Combinacion</t>
+  </si>
+  <si>
+    <t>Señal de datos</t>
+  </si>
+  <si>
+    <t>Comunicación</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>Ejemplo</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Caracteristica</t>
+  </si>
+  <si>
+    <t>Problematicas</t>
+  </si>
+  <si>
+    <t>Colision</t>
+  </si>
+  <si>
+    <t>EMI</t>
+  </si>
+  <si>
+    <t>RFI</t>
+  </si>
+  <si>
+    <t>Crosstalk</t>
+  </si>
+  <si>
+    <t>concepto</t>
+  </si>
+  <si>
+    <t>Interf. Electromagnetica</t>
+  </si>
+  <si>
+    <t>Interf. Radiofrecuencia</t>
+  </si>
+  <si>
+    <t>Choque de señales</t>
+  </si>
+  <si>
+    <t>Diafonia (Cruce de Señales)</t>
   </si>
 </sst>
 </file>
@@ -145,7 +621,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,6 +674,54 @@
       <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -293,7 +817,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -301,60 +825,108 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -364,24 +936,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,6 +961,301 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>676603</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>65690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>52552</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>105103</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector recto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32727137-50B5-482B-A31C-6728143F0830}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="676603" y="446690"/>
+          <a:ext cx="1090449" cy="420413"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>893379</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85397</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19707</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>78828</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Conector recto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B141DB6-4C97-437F-ABC0-0E5A43E2371F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="893379" y="656897"/>
+          <a:ext cx="1083880" cy="755431"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>873672</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>65691</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>39414</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>105103</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Conector recto 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECF7F045-6944-4575-9402-C2BED59B525F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="873672" y="637191"/>
+          <a:ext cx="1123294" cy="801412"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>702879</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>91966</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>39414</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>111673</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F2634D3-8758-4FC9-856B-B2763CB6575B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="702879" y="472966"/>
+          <a:ext cx="1051035" cy="400707"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="accent2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9CCDC61-9019-4C6D-A06B-84D29AFEF12E}" name="Tabla1" displayName="Tabla1" ref="A4:C16" totalsRowShown="0">
+  <autoFilter ref="A4:C16" xr:uid="{A9CCDC61-9019-4C6D-A06B-84D29AFEF12E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{CB3D0213-9198-4683-B7C1-367F28FAF5B8}" name="unidad"/>
+    <tableColumn id="2" xr3:uid="{2FB2436F-D1D1-443E-9C8C-2F1976A69FE5}" name="equivalencia"/>
+    <tableColumn id="3" xr3:uid="{64D03617-DCEB-4482-9AE5-836C2721FA61}" name="exponente"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6C6D8F50-DDEA-4CB6-AECB-C91F008AE46E}" name="Tabla2" displayName="Tabla2" ref="E4:G9" totalsRowShown="0">
+  <autoFilter ref="E4:G9" xr:uid="{6C6D8F50-DDEA-4CB6-AECB-C91F008AE46E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B51E7C21-FDAF-477B-846F-996E4C3C7EB7}" name="unidad"/>
+    <tableColumn id="2" xr3:uid="{51796D62-F59D-489C-AD02-690905E2A781}" name="equivalencia"/>
+    <tableColumn id="3" xr3:uid="{F77F5CAD-ED39-4836-B01B-748E6CE3B421}" name="exponencia"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{09807BD8-AA50-4C29-ACE1-024E25517512}" name="Tabla3" displayName="Tabla3" ref="E12:G16" totalsRowShown="0">
+  <autoFilter ref="E12:G16" xr:uid="{09807BD8-AA50-4C29-ACE1-024E25517512}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A648E674-05A7-4EF3-A1D7-2B08FF6E0945}" name="hertz"/>
+    <tableColumn id="2" xr3:uid="{62AB139A-7590-4730-8946-70A55EE1B689}" name="1 ciclo/s"/>
+    <tableColumn id="3" xr3:uid="{2D13D491-A241-4CCA-85FF-0D819173C5CD}" name="10^0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BF72E9EB-D48A-408F-A2C6-1CBD103DC7EE}" name="Tabla4" displayName="Tabla4" ref="A12:C16" totalsRowShown="0">
+  <autoFilter ref="A12:C16" xr:uid="{BF72E9EB-D48A-408F-A2C6-1CBD103DC7EE}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{EC007214-F660-4460-99F1-62FBA952AD8E}" name="Comunicación"/>
+    <tableColumn id="2" xr3:uid="{9F87449E-8FF0-48CA-9753-A93E75D939A2}" name="Concepto"/>
+    <tableColumn id="3" xr3:uid="{2F049624-BAE5-4D36-9C6E-C2805CABFE09}" name="Ejemplo"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D1FAACFE-2D97-4741-9C70-4BE5DBBE88C8}" name="Tabla5" displayName="Tabla5" ref="E12:G16" totalsRowShown="0">
+  <autoFilter ref="E12:G16" xr:uid="{D1FAACFE-2D97-4741-9C70-4BE5DBBE88C8}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{215CBA66-5A27-49CE-AC03-00432E7F3317}" name="Tipo"/>
+    <tableColumn id="2" xr3:uid="{92E3B12E-C627-473A-9C3C-D59CEF165866}" name="Concepto"/>
+    <tableColumn id="3" xr3:uid="{06CDA896-BA05-4A85-82AA-E3466E50A7ED}" name="Caracteristica"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -703,7 +1557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE91CD09-8D46-4150-91A3-935B67F81363}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -716,102 +1570,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="34" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="7"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="35"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="20"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="36"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="16" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="18" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="37" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="14"/>
+      <c r="D8" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -824,4 +1678,691 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D646EF-9814-4598-80CC-989625FE9413}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="E3" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E11:G11"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140058D3-1D45-406D-8302-57E7EE53FED0}">
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I2" s="43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" t="s">
+        <v>153</v>
+      </c>
+      <c r="J3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4" t="s">
+        <v>152</v>
+      </c>
+      <c r="J4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6" t="s">
+        <v>150</v>
+      </c>
+      <c r="J6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" s="43" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" t="s">
+        <v>137</v>
+      </c>
+      <c r="I8" t="s">
+        <v>154</v>
+      </c>
+      <c r="J8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9" t="s">
+        <v>137</v>
+      </c>
+      <c r="G9" t="s">
+        <v>136</v>
+      </c>
+      <c r="I9" t="s">
+        <v>155</v>
+      </c>
+      <c r="J9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I10" t="s">
+        <v>156</v>
+      </c>
+      <c r="J10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F12" t="s">
+        <v>169</v>
+      </c>
+      <c r="G12" t="s">
+        <v>172</v>
+      </c>
+      <c r="I12" t="s">
+        <v>173</v>
+      </c>
+      <c r="J12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" t="s">
+        <v>167</v>
+      </c>
+      <c r="I13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" t="s">
+        <v>164</v>
+      </c>
+      <c r="I14" t="s">
+        <v>175</v>
+      </c>
+      <c r="J14" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G15" t="s">
+        <v>165</v>
+      </c>
+      <c r="I15" t="s">
+        <v>176</v>
+      </c>
+      <c r="J15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" t="s">
+        <v>121</v>
+      </c>
+      <c r="G16" t="s">
+        <v>166</v>
+      </c>
+      <c r="I16" t="s">
+        <v>177</v>
+      </c>
+      <c r="J16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="2">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Capa Fisica: Fibra Optica
</commit_message>
<xml_diff>
--- a/docs/protocols-suite.xlsx
+++ b/docs/protocols-suite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna1-mj20\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE3FFCF-5BB8-45A0-8702-C194A7BEAE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED159B3-6E9D-455C-9467-9D1EA6723CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{61336F32-1C3D-4908-AE32-B989E9366DB6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="182">
   <si>
     <t>OSI de ISO</t>
   </si>
@@ -482,12 +482,6 @@
     <t>Fibra</t>
   </si>
   <si>
-    <t>conectores</t>
-  </si>
-  <si>
-    <t>terminaciones</t>
-  </si>
-  <si>
     <t>ST</t>
   </si>
   <si>
@@ -509,27 +503,6 @@
     <t>APC</t>
   </si>
   <si>
-    <t>Suscriber Connector</t>
-  </si>
-  <si>
-    <t>Ferrule Conector</t>
-  </si>
-  <si>
-    <t>Lucent Conector</t>
-  </si>
-  <si>
-    <t>Straight Tip</t>
-  </si>
-  <si>
-    <t>Physical Contact</t>
-  </si>
-  <si>
-    <t>Angled Physical Contact</t>
-  </si>
-  <si>
-    <t>Ultra Physical Contact</t>
-  </si>
-  <si>
     <t>Largo de la Onda</t>
   </si>
   <si>
@@ -572,9 +545,6 @@
     <t>Crosstalk</t>
   </si>
   <si>
-    <t>concepto</t>
-  </si>
-  <si>
     <t>Interf. Electromagnetica</t>
   </si>
   <si>
@@ -585,6 +555,33 @@
   </si>
   <si>
     <t>Diafonia (Cruce de Señales)</t>
+  </si>
+  <si>
+    <t>Terminaciones</t>
+  </si>
+  <si>
+    <t>Conectores</t>
+  </si>
+  <si>
+    <t>SC (Suscriptor Connector)</t>
+  </si>
+  <si>
+    <t>LC (Lucent Connector)</t>
+  </si>
+  <si>
+    <t>FC (Ferrule Connector)</t>
+  </si>
+  <si>
+    <t>ST (Straight Connector)</t>
+  </si>
+  <si>
+    <t>PC  (Physical Contact)</t>
+  </si>
+  <si>
+    <t>UPC (Ultra Physical Contact)</t>
+  </si>
+  <si>
+    <t>APC (Angled Physical Contact)</t>
   </si>
 </sst>
 </file>
@@ -621,7 +618,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -724,8 +721,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -813,11 +840,88 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -941,6 +1045,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1253,6 +1390,18 @@
     <tableColumn id="1" xr3:uid="{215CBA66-5A27-49CE-AC03-00432E7F3317}" name="Tipo"/>
     <tableColumn id="2" xr3:uid="{92E3B12E-C627-473A-9C3C-D59CEF165866}" name="Concepto"/>
     <tableColumn id="3" xr3:uid="{06CDA896-BA05-4A85-82AA-E3466E50A7ED}" name="Caracteristica"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{820F069F-2F93-4970-ACF5-ED4D020D55E9}" name="Tabla7" displayName="Tabla7" ref="E2:G10" totalsRowShown="0">
+  <autoFilter ref="E2:G10" xr:uid="{820F069F-2F93-4970-ACF5-ED4D020D55E9}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{5011CCA9-4806-432C-A340-C02034BE57B9}" name="Fibra"/>
+    <tableColumn id="2" xr3:uid="{00A4589F-A8D1-4DA8-B127-91B1BD13348F}" name="SMF(Single Mode)"/>
+    <tableColumn id="3" xr3:uid="{19772779-4611-439E-A990-B7A6B47AAF85}" name="MMF (MultiMode)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1985,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{140058D3-1D45-406D-8302-57E7EE53FED0}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1995,10 +2144,10 @@
     <col min="2" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
     <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
     <col min="8" max="8" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2025,9 +2174,10 @@
       <c r="G2" t="s">
         <v>146</v>
       </c>
-      <c r="I2" s="43" t="s">
-        <v>148</v>
-      </c>
+      <c r="I2" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="J2" s="52"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
@@ -2048,11 +2198,11 @@
       <c r="G3" t="s">
         <v>124</v>
       </c>
-      <c r="I3" t="s">
-        <v>153</v>
-      </c>
-      <c r="J3" t="s">
-        <v>157</v>
+      <c r="I3" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="J3" s="53" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2074,11 +2224,11 @@
       <c r="G4" t="s">
         <v>126</v>
       </c>
-      <c r="I4" t="s">
-        <v>152</v>
-      </c>
-      <c r="J4" t="s">
-        <v>158</v>
+      <c r="I4" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2100,11 +2250,11 @@
       <c r="G5" t="s">
         <v>130</v>
       </c>
-      <c r="I5" t="s">
-        <v>151</v>
-      </c>
-      <c r="J5" t="s">
-        <v>159</v>
+      <c r="I5" s="55" t="s">
+        <v>149</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2124,11 +2274,11 @@
       <c r="G6" t="s">
         <v>139</v>
       </c>
-      <c r="I6" t="s">
-        <v>150</v>
-      </c>
-      <c r="J6" t="s">
-        <v>160</v>
+      <c r="I6" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="J6" s="56" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2148,9 +2298,10 @@
       <c r="G7" t="s">
         <v>133</v>
       </c>
-      <c r="I7" s="43" t="s">
-        <v>149</v>
-      </c>
+      <c r="I7" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="J7" s="52"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
@@ -2171,11 +2322,11 @@
       <c r="G8" t="s">
         <v>137</v>
       </c>
-      <c r="I8" t="s">
-        <v>154</v>
-      </c>
-      <c r="J8" t="s">
-        <v>161</v>
+      <c r="I8" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="J8" s="57" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2195,14 +2346,14 @@
       <c r="G9" t="s">
         <v>136</v>
       </c>
-      <c r="I9" t="s">
-        <v>155</v>
-      </c>
-      <c r="J9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="58" t="s">
+        <v>153</v>
+      </c>
+      <c r="J9" s="58" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
         <v>99</v>
       </c>
@@ -2219,38 +2370,36 @@
       <c r="G10" t="s">
         <v>143</v>
       </c>
-      <c r="I10" t="s">
-        <v>156</v>
-      </c>
-      <c r="J10" t="s">
-        <v>162</v>
+      <c r="I10" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="J10" s="59" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C12" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="E12" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="F12" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="G12" t="s">
-        <v>172</v>
-      </c>
-      <c r="I12" t="s">
-        <v>173</v>
-      </c>
-      <c r="J12" t="s">
-        <v>178</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="I12" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="J12" s="52"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2269,13 +2418,13 @@
         <v>122</v>
       </c>
       <c r="G13" t="s">
-        <v>167</v>
-      </c>
-      <c r="I13" t="s">
-        <v>174</v>
-      </c>
-      <c r="J13" t="s">
-        <v>181</v>
+        <v>158</v>
+      </c>
+      <c r="I13" s="47" t="s">
+        <v>165</v>
+      </c>
+      <c r="J13" s="48" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2295,13 +2444,13 @@
         <v>119</v>
       </c>
       <c r="G14" t="s">
-        <v>164</v>
-      </c>
-      <c r="I14" t="s">
-        <v>175</v>
-      </c>
-      <c r="J14" t="s">
-        <v>179</v>
+        <v>155</v>
+      </c>
+      <c r="I14" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14" s="50" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2321,13 +2470,13 @@
         <v>120</v>
       </c>
       <c r="G15" t="s">
-        <v>165</v>
-      </c>
-      <c r="I15" t="s">
-        <v>176</v>
-      </c>
-      <c r="J15" t="s">
-        <v>180</v>
+        <v>156</v>
+      </c>
+      <c r="I15" s="47" t="s">
+        <v>167</v>
+      </c>
+      <c r="J15" s="48" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2347,22 +2496,28 @@
         <v>121</v>
       </c>
       <c r="G16" t="s">
-        <v>166</v>
-      </c>
-      <c r="I16" t="s">
-        <v>177</v>
-      </c>
-      <c r="J16" t="s">
-        <v>182</v>
+        <v>157</v>
+      </c>
+      <c r="I16" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="J16" s="46" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I2:J2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>